<commit_message>
Adding ppkt for NUP210L
</commit_message>
<xml_diff>
--- a/notebooks/AAGAB/input/AAGAB_PPKP1A_individuals.xlsx
+++ b/notebooks/AAGAB/input/AAGAB_PPKP1A_individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/GIT/phenopacket-store/notebooks/AAGAB/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A5757B-9A70-BA4A-BD64-E03D1EFF1459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5B7C16-5B01-2745-81EB-5BAAECB646CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9280" yWindow="10360" windowWidth="27000" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="6740" windowWidth="27000" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -136,9 +136,6 @@
     <t>HP:0006482</t>
   </si>
   <si>
-    <t>Abnormality of the nail</t>
-  </si>
-  <si>
     <t>HP:0001597</t>
   </si>
   <si>
@@ -191,6 +188,9 @@
   </si>
   <si>
     <t>Abnormal hair morphology</t>
+  </si>
+  <si>
+    <t>Abnormal nail morphology</t>
   </si>
 </sst>
 </file>
@@ -564,7 +564,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -625,13 +625,13 @@
         <v>35</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -693,10 +693,10 @@
         <v>37</v>
       </c>
       <c r="T2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" t="s">
         <v>39</v>
-      </c>
-      <c r="U2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -726,16 +726,16 @@
         <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K3" t="s">
         <v>28</v>
       </c>
       <c r="L3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N3" t="s">
         <v>32</v>
@@ -750,16 +750,16 @@
         <v>28</v>
       </c>
       <c r="R3" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" t="s">
         <v>41</v>
       </c>
-      <c r="S3" t="s">
-        <v>42</v>
-      </c>
       <c r="T3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -770,7 +770,7 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
@@ -788,19 +788,19 @@
         <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K4" t="s">
         <v>28</v>
       </c>
       <c r="L4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O4" t="s">
         <v>33</v>
@@ -812,16 +812,16 @@
         <v>28</v>
       </c>
       <c r="R4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -832,7 +832,7 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -850,19 +850,19 @@
         <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s">
         <v>28</v>
       </c>
       <c r="L5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" t="s">
         <v>52</v>
-      </c>
-      <c r="M5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N5" t="s">
-        <v>53</v>
       </c>
       <c r="O5" t="s">
         <v>33</v>
@@ -874,16 +874,16 @@
         <v>28</v>
       </c>
       <c r="R5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>